<commit_message>
resolved :   error  not printing out the first class
</commit_message>
<xml_diff>
--- a/preachersDb.xlsx
+++ b/preachersDb.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alliance/PycharmProjects/timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC446537-228B-C646-9DB0-D33D209A8ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01218C9-2B53-5D4B-A5C6-A27F2F519CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="preachers" sheetId="1" r:id="rId1"/>
+    <sheet name="testData" sheetId="1" r:id="rId1"/>
+    <sheet name="preachers" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="100">
   <si>
     <t>PREACHERS LIST</t>
   </si>
@@ -197,13 +198,136 @@
   </si>
   <si>
     <t>cameron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carine &amp; bayigamba </t>
+  </si>
+  <si>
+    <t>calvin &amp; flower</t>
+  </si>
+  <si>
+    <t>rwabigwi annette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethan &amp; shania </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cyuzuzo &amp; chris </t>
+  </si>
+  <si>
+    <t>boaz &amp; debora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maeva &amp; clelia </t>
+  </si>
+  <si>
+    <t>doriane &amp; carly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anais &amp; keysha </t>
+  </si>
+  <si>
+    <t>Keyla &amp; shilah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angel &amp; Honest </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elijah &amp; kenny </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ketty &amp; shania </t>
+  </si>
+  <si>
+    <t>sasha juliene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anitha &amp; hope </t>
+  </si>
+  <si>
+    <t xml:space="preserve">solange &amp; nice </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kelsy &amp; kestia </t>
+  </si>
+  <si>
+    <t>iza &amp; mbaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aliane &amp; yakine </t>
+  </si>
+  <si>
+    <t>gloria &amp; noella</t>
+  </si>
+  <si>
+    <t>nelsi &amp; keysie</t>
+  </si>
+  <si>
+    <t>emma &amp; shaun</t>
+  </si>
+  <si>
+    <t>queen &amp; eugene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gaella &amp; hope </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nick &amp; atfa </t>
+  </si>
+  <si>
+    <t>olga &amp; lilian</t>
+  </si>
+  <si>
+    <t>jeremy &amp; samuella</t>
+  </si>
+  <si>
+    <t>pamela &amp; nancy</t>
+  </si>
+  <si>
+    <t>mugunga &amp; ndahiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tunga &amp; evlyne </t>
+  </si>
+  <si>
+    <t>alicia &amp; chanella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celia &amp; chelsea </t>
+  </si>
+  <si>
+    <t>y11,y12,y13</t>
+  </si>
+  <si>
+    <t>y11,y13</t>
+  </si>
+  <si>
+    <t>y13,y12</t>
+  </si>
+  <si>
+    <t>zumpire &amp; queen linda</t>
+  </si>
+  <si>
+    <t>Nshuti Lincoln</t>
+  </si>
+  <si>
+    <t>kenny &amp; elijah</t>
+  </si>
+  <si>
+    <t>angella &amp; keren</t>
+  </si>
+  <si>
+    <t>ketty &amp; nailla</t>
+  </si>
+  <si>
+    <t>gahima &amp; peace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +348,33 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -246,14 +397,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A1:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -571,15 +732,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1036,4 +1197,671 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5B239-7DF4-6C4A-8CD6-F9E721F3962B}">
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="65" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a workbook for testing
</commit_message>
<xml_diff>
--- a/preachersDb.xlsx
+++ b/preachersDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alliance/PycharmProjects/timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01218C9-2B53-5D4B-A5C6-A27F2F519CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7D2A63-5860-7744-8D69-2DEE4284A39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5B239-7DF4-6C4A-8CD6-F9E721F3962B}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>